<commit_message>
finished Tim McGraw data
</commit_message>
<xml_diff>
--- a/proposal/Data/Tim McGraw.xlsx
+++ b/proposal/Data/Tim McGraw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmagraebner/Desktop/course-paper-or-presentation-emmagraebner/proposal/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE5F2AF6-132F-A640-B164-8A5EE898B06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E52854-D132-C84E-A5B6-0BB721FCEA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{46E66E81-EF18-D44C-8EC5-7DB50ED4E92A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{46E66E81-EF18-D44C-8EC5-7DB50ED4E92A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="128">
   <si>
     <t>I</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>that's</t>
+  </si>
+  <si>
+    <t>305/362</t>
+  </si>
+  <si>
+    <t>Proportion Repeated</t>
   </si>
 </sst>
 </file>
@@ -778,18 +784,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC1F4E1-6435-A04B-B5D2-FFA522BF903B}">
-  <dimension ref="A1:C362"/>
+  <dimension ref="A1:D362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -799,8 +806,11 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -810,8 +820,11 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -822,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -833,7 +846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -844,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -855,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -866,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -877,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -888,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -899,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -910,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -921,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -932,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -943,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -954,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>